<commit_message>
Facilitating a bigger split between races
</commit_message>
<xml_diff>
--- a/TORX DUV dates/TORX_duv_dates_df.xlsx
+++ b/TORX DUV dates/TORX_duv_dates_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
   <si>
     <t>Race</t>
   </si>
@@ -28,42 +28,36 @@
     <t>Day_of_Week Start_Date</t>
   </si>
   <si>
-    <t>TOR130</t>
-  </si>
-  <si>
     <t>TOR330</t>
   </si>
   <si>
-    <t>TOR450</t>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2017</t>
   </si>
   <si>
     <t>2024</t>
   </si>
   <si>
-    <t>2023</t>
+    <t>2013</t>
   </si>
   <si>
     <t>2022</t>
   </si>
   <si>
+    <t>2014</t>
+  </si>
+  <si>
     <t>2019</t>
   </si>
   <si>
     <t>2018</t>
   </si>
   <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2021</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
     <t>2016</t>
   </si>
   <si>
@@ -79,16 +73,7 @@
     <t>2010</t>
   </si>
   <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
     <t>Sunday</t>
-  </si>
-  <si>
-    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -450,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -475,13 +460,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2">
-        <v>45545.875</v>
+        <v>45179.41666666666</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -489,13 +474,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>45181.875</v>
+        <v>44451.41666666666</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -503,13 +488,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
-        <v>44817.875</v>
+        <v>42988.41666666666</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -517,13 +502,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
-        <v>43718.875</v>
+        <v>45543.41666666666</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -531,13 +516,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
-        <v>43354.875</v>
+        <v>41525.41666666666</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -545,13 +530,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2">
-        <v>42991.875</v>
+        <v>44815.41666666666</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -559,279 +544,111 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2">
-        <v>44453.875</v>
+        <v>41889.41666666666</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
-        <v>45179.41666666666</v>
+        <v>43716.41666666666</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2">
-        <v>44451.41666666666</v>
+        <v>43352.41666666666</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
-        <v>42988.41666666666</v>
+        <v>42624.41666666666</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2">
-        <v>45543.41666666666</v>
+        <v>41161.41666666666</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C13" s="2">
-        <v>41525.41666666666</v>
+        <v>40797.41666666666</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2">
-        <v>44815.41666666666</v>
+        <v>42260.41666666666</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2">
-        <v>41889.41666666666</v>
+        <v>40433.41666666666</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="2">
-        <v>43716.41666666666</v>
-      </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="2">
-        <v>43352.41666666666</v>
-      </c>
-      <c r="D17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2">
-        <v>42624.41666666666</v>
-      </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="2">
-        <v>41161.41666666666</v>
-      </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="2">
-        <v>40797.41666666666</v>
-      </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="2">
-        <v>42260.41666666666</v>
-      </c>
-      <c r="D21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="2">
-        <v>40433.41666666666</v>
-      </c>
-      <c r="D22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="2">
-        <v>45177.83333333334</v>
-      </c>
-      <c r="D23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="2">
-        <v>45541.83333333334</v>
-      </c>
-      <c r="D24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="2">
-        <v>44813.83333333334</v>
-      </c>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="2">
-        <v>43714.83333333334</v>
-      </c>
-      <c r="D26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="2">
-        <v>44449.83333333334</v>
-      </c>
-      <c r="D27" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Saving automatically for each race
</commit_message>
<xml_diff>
--- a/TORX DUV dates/TORX_duv_dates_df.xlsx
+++ b/TORX DUV dates/TORX_duv_dates_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="25">
   <si>
     <t>Race</t>
   </si>
@@ -28,36 +28,42 @@
     <t>Day_of_Week Start_Date</t>
   </si>
   <si>
+    <t>TOR130</t>
+  </si>
+  <si>
     <t>TOR330</t>
   </si>
   <si>
+    <t>TOR450</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
     <t>2023</t>
   </si>
   <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
     <t>2021</t>
   </si>
   <si>
-    <t>2017</t>
-  </si>
-  <si>
-    <t>2024</t>
-  </si>
-  <si>
     <t>2013</t>
   </si>
   <si>
-    <t>2022</t>
-  </si>
-  <si>
     <t>2014</t>
   </si>
   <si>
-    <t>2019</t>
-  </si>
-  <si>
-    <t>2018</t>
-  </si>
-  <si>
     <t>2016</t>
   </si>
   <si>
@@ -73,7 +79,16 @@
     <t>2010</t>
   </si>
   <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
     <t>Sunday</t>
+  </si>
+  <si>
+    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -435,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,13 +475,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2">
-        <v>45179.41666666666</v>
+        <v>45545.875</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -474,13 +489,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
-        <v>44451.41666666666</v>
+        <v>45181.875</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -488,13 +503,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
-        <v>42988.41666666666</v>
+        <v>44817.875</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -502,13 +517,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
-        <v>45543.41666666666</v>
+        <v>43718.875</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -516,13 +531,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>41525.41666666666</v>
+        <v>43354.875</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -530,13 +545,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
-        <v>44815.41666666666</v>
+        <v>42991.875</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -544,111 +559,279 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
-        <v>41889.41666666666</v>
+        <v>44453.875</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>43716.41666666666</v>
+        <v>45179.41666666666</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2">
-        <v>43352.41666666666</v>
+        <v>44451.41666666666</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C11" s="2">
-        <v>42624.41666666666</v>
+        <v>42988.41666666666</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2">
-        <v>41161.41666666666</v>
+        <v>45543.41666666666</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2">
-        <v>40797.41666666666</v>
+        <v>41525.41666666666</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2">
-        <v>42260.41666666666</v>
+        <v>44815.41666666666</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="2">
+        <v>41889.41666666666</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43716.41666666666</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43352.41666666666</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2">
+        <v>42624.41666666666</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2">
+        <v>41161.41666666666</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C20" s="2">
+        <v>40797.41666666666</v>
+      </c>
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2">
+        <v>42260.41666666666</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
         <v>40433.41666666666</v>
       </c>
-      <c r="D15" t="s">
-        <v>19</v>
+      <c r="D22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2">
+        <v>45177.83333333334</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2">
+        <v>45541.83333333334</v>
+      </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2">
+        <v>44813.83333333334</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2">
+        <v>43714.83333333334</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="2">
+        <v>44449.83333333334</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>